<commit_message>
Changed TCXO->MEMS TCXO. BOM finished
</commit_message>
<xml_diff>
--- a/Sch/adc/zturn_adc.xlsx
+++ b/Sch/adc/zturn_adc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="172">
   <si>
     <t xml:space="preserve"> Value</t>
   </si>
@@ -57,54 +57,24 @@
     <t>Header5</t>
   </si>
   <si>
-    <t>RN1</t>
-  </si>
-  <si>
-    <t>RN2</t>
-  </si>
-  <si>
-    <t>RN3</t>
-  </si>
-  <si>
-    <t>RN4</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
-    <t>RN5</t>
-  </si>
-  <si>
-    <t>W1</t>
-  </si>
-  <si>
     <t>TEST_1P</t>
   </si>
   <si>
-    <t>W2</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>BGA2818</t>
   </si>
   <si>
     <t>22nF</t>
   </si>
   <si>
-    <t>L2</t>
-  </si>
-  <si>
     <t>220nH</t>
   </si>
   <si>
     <t>18p</t>
   </si>
   <si>
-    <t>L4</t>
-  </si>
-  <si>
     <t>L3</t>
   </si>
   <si>
@@ -126,51 +96,24 @@
     <t>X1</t>
   </si>
   <si>
-    <t>ECS-TXO-2520</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
-    <t>L6</t>
-  </si>
-  <si>
     <t>JP2</t>
   </si>
   <si>
     <t>0.1uF</t>
   </si>
   <si>
-    <t>C6</t>
-  </si>
-  <si>
     <t>12pF</t>
   </si>
   <si>
-    <t>CN1</t>
-  </si>
-  <si>
     <t>SMA</t>
   </si>
   <si>
-    <t>CN2</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
@@ -180,9 +123,6 @@
     <t>C19</t>
   </si>
   <si>
-    <t>L9</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -207,9 +147,6 @@
     <t>4.7uF</t>
   </si>
   <si>
-    <t>L8</t>
-  </si>
-  <si>
     <t>Part</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -254,26 +191,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>GRM188R61C225KE15D</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>490-3296-1-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>10nF</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>GRM188R71H103KA01D</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>490-1512-1-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>GRM188R71C104KA01D</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -302,13 +219,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>0.1uFに変更</t>
-    <rPh sb="6" eb="8">
-      <t>ヘンコウ</t>
-    </rPh>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>0402</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -325,10 +235,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>2.2uF</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>0402</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -358,13 +264,6 @@
   </si>
   <si>
     <t>C6,C31,C32,C40</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>0402に変更</t>
-    <rPh sb="5" eb="7">
-      <t>ヘンコウ</t>
-    </rPh>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -521,44 +420,253 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>R1,R2,R3,R9,R10,R11R21,
+    <t>ERJ-3EKF22R0V</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P22.0HCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>R15,R29,R30</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ERJ-3EKF51R0V</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ERJ-3EKF24R9V</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P24.9HCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>P51.0HCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>R7,R8,R17,R18,R19,R20</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>R4,R12,R13,R14</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>LTC2292CUP#PBF</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Linear Technology</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>LTC2292CUP#PBF-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1206</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>EXB-38V220JV</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Y9220CT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>RN1,RN2,RN3,RN4,RN5</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>BGA2818,115</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>NXP USA Inc.</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>568-12531-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>U2,U4</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>MABAES0060</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>M/A-Com Technology Solutions</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1465-1317-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>R1,R2,R9,R10,R11R21,
 R22,R23,R27,R28</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>ERJ-3EKF22R0V</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P22.0HCT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>R15,R29,R30</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>ERJ-3EKF51R0V</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>ERJ-3EKF24R9V</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P24.9HCT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>P51.0HCT-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>R7,R8,R17,R18,R19,R20</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>R4,R12,R13,R14</t>
+    <t>SIT5001</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SIT5001AC-3E-33N0-40.000000X</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SiTIME</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1473-1518-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>5-1814400-1</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>TE Connectivity AMP Connectors</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>A97593-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>CN1,CN2</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>CDCLVC1102PWR</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>296-27610-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>TLV70230DBVR</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>296-39283-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>NAU8822LYG</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Nuvoton Technology Corporation
+of America</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>NAU8822LYG-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SJ-3523-SMT-TR</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>CUI Inc.</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>CP-3523SJCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>L2,L4</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>MLF1608DR22JTD25</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>TDK Corporation</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>445-16955-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>HK060327NJ-T</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>587-1490-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>20021121-00080T4LF</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Amphenol FCI</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>609-3741-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>MPZ2012S601AT000</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>TDK Corporation</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>445-2206-1-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>0805</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>L1,L5,L6,L8,L9</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>68000-401HLF</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Amphenol FCI</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>609-3466-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>W1,W2</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -736,7 +844,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -914,12 +1022,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1167,7 +1269,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1176,12 +1278,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1507,43 +1603,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="D1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1554,6 +1650,15 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1562,22 +1667,31 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1588,13 +1702,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1605,610 +1719,591 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="B7">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>22</v>
+      <c r="C7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="B9">
         <v>22</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>139</v>
+        <v>171</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" t="s">
+        <v>169</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>131</v>
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>22</v>
+        <v>153</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13">
-        <v>22</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>130</v>
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
+        <v>117</v>
+      </c>
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="C22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E31" t="s">
+        <v>139</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B21">
-        <v>25</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="D32" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="E21" t="s">
-        <v>136</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22">
-        <v>50</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E22" t="s">
-        <v>136</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" t="s">
-        <v>102</v>
-      </c>
-      <c r="E31" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>98</v>
-      </c>
-      <c r="B32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" t="s">
-        <v>84</v>
+        <v>35</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="E33" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" t="s">
-        <v>88</v>
-      </c>
-      <c r="E34" t="s">
-        <v>67</v>
+        <v>37</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" t="s">
-        <v>106</v>
+        <v>39</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="E35" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D36" t="s">
-        <v>111</v>
+        <v>166</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="E36" t="s">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>112</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37" t="s">
-        <v>67</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>117</v>
-      </c>
-      <c r="B38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D38" t="s">
-        <v>113</v>
-      </c>
-      <c r="E38" t="s">
-        <v>67</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>121</v>
-      </c>
-      <c r="B39" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E39" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>138</v>
-      </c>
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D41" t="s">
-        <v>135</v>
-      </c>
-      <c r="E41" t="s">
-        <v>136</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>142</v>
-      </c>
-      <c r="B50" t="s">
-        <v>134</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>62</v>
-      </c>
-      <c r="B51" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done except GND net
</commit_message>
<xml_diff>
--- a/Sch/adc/zturn_adc.xlsx
+++ b/Sch/adc/zturn_adc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16188" windowHeight="9912"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11820" windowHeight="9912"/>
   </bookViews>
   <sheets>
     <sheet name="zturn_adc" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="171">
   <si>
     <t xml:space="preserve"> Value</t>
   </si>
@@ -120,9 +120,6 @@
     <t>CDCLVC1102</t>
   </si>
   <si>
-    <t>C19</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -155,10 +152,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>GRM188R61A105KA61D</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>Manufacturer</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -167,10 +160,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>C1,C2</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>0603</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -187,10 +176,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>490-1543-1-ND</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>GRM188R71C104KA01D</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -340,10 +325,6 @@
   </si>
   <si>
     <t>C21,C27</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>J3,J4,J5,J6,J7</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -624,10 +605,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>L1,L5,L6,L8,L9</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>68000-401HLF</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -669,12 +646,24 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>R2,R9,R10,R11R21,
+    <t>R1,R4,R12,R13,R14</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>J3,J4,J5,J6</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>C1,C2,C19,C48,C49</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>R2,R3,R9,R10,R11R21,
 R22,R23,R27,R28</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>R1,R4,R12,R13,R14</t>
+    <t>L1,L5,L6,L7,L8,L9,L10,L11</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -1611,10 +1600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1630,7 +1619,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1639,13 +1628,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
@@ -1659,13 +1648,13 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1676,30 +1665,30 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1710,13 +1699,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1727,113 +1716,113 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B7">
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B9">
         <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B10">
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" t="s">
         <v>99</v>
       </c>
-      <c r="D11" t="s">
-        <v>104</v>
-      </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1844,70 +1833,70 @@
         <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E13" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E15" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1918,36 +1907,36 @@
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E16" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1958,13 +1947,13 @@
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E18" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1972,216 +1961,216 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E19" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
         <v>47</v>
       </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
         <v>49</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>170</v>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>168</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E24" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
         <v>57</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2189,16 +2178,16 @@
         <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
         <v>84</v>
       </c>
       <c r="E30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>85</v>
@@ -2206,118 +2195,98 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" t="s">
-        <v>88</v>
+        <v>30</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="E31" t="s">
-        <v>46</v>
+        <v>130</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" t="s">
         <v>134</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>134</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="1" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E34" t="s">
-        <v>139</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="E35" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E36" t="s">
-        <v>147</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>110</v>
-      </c>
-      <c r="B37" t="s">
-        <v>103</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed to SMD type. Update BOM
</commit_message>
<xml_diff>
--- a/Sch/adc/zturn_adc.xlsx
+++ b/Sch/adc/zturn_adc.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11820" windowHeight="9912"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25572" windowHeight="8508"/>
   </bookViews>
   <sheets>
     <sheet name="zturn_adc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="182">
   <si>
     <t xml:space="preserve"> Value</t>
   </si>
@@ -27,9 +27,6 @@
     <t xml:space="preserve"> Footprint</t>
   </si>
   <si>
-    <t xml:space="preserve"> Datasheet</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>X1</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>12pF</t>
   </si>
   <si>
-    <t>SMA</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
@@ -145,10 +136,6 @@
   </si>
   <si>
     <t>Part</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Digikey</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -658,12 +645,72 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>R2,R3,R9,R10,R11R21,
+    <t>L1,L5,L6,L7,L8,L9,L10,L11</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>QFN</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SMD</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Take care of rotation</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Mount towards outside of the PCB</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Digikey Part Number</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>PTH</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>R2,R3,R9,R10,R11,R21,
 R22,R23,R27,R28</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>L1,L5,L6,L7,L8,L9,L10,L11</t>
+    <t xml:space="preserve">Mount Top Side </t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Mount Bottom Side</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SMD Parts Count</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>C4,C40,C46,C47,C53</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>All the other</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SMA Connector</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Ferite Bead</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -1022,7 +1069,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1137,6 +1184,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1266,18 +1358,48 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1600,693 +1722,987 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="34.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="7">
+        <v>22</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="7">
+        <v>22</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="7">
+        <v>25</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="7">
+        <v>50</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="F22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="3" t="s">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I32" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I33" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I34" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38">
+        <v>98</v>
+      </c>
+      <c r="C38" t="s">
+        <v>179</v>
+      </c>
+      <c r="I38" s="13" t="str">
+        <f>"Total: " &amp; SUM(I2:I36)</f>
+        <v>Total: 103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B9">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>159</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E13" t="s">
-        <v>157</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" t="s">
-        <v>119</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E15" t="s">
-        <v>146</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E16" t="s">
-        <v>148</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" t="s">
-        <v>123</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E19" t="s">
-        <v>127</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>168</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>132</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E31" t="s">
-        <v>130</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E32" t="s">
-        <v>134</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E33" t="s">
-        <v>134</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E35" t="s">
-        <v>142</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>105</v>
-      </c>
-      <c r="B36" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>94</v>
+      <c r="C39" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed some resistors to 0402.
</commit_message>
<xml_diff>
--- a/Sch/adc/zturn_adc.xlsx
+++ b/Sch/adc/zturn_adc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="224">
   <si>
     <t xml:space="preserve"> Value</t>
   </si>
@@ -678,11 +678,6 @@
   </si>
   <si>
     <t>PTH</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>R2,R3,R9,R10,R11,R21,
-R22,R23,R27,R28</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -868,6 +863,14 @@
   </si>
   <si>
     <t>10k Ohm ±1% 0.1W, 1/10W Chip Resistor 0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>R21,R22,R23</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>R2,R3,R9,R10,R11,R27,R28</t>
+    <phoneticPr fontId="18"/>
   </si>
 </sst>
 </file>
@@ -1883,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1924,13 +1927,13 @@
         <v>172</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1954,7 +1957,7 @@
         <v>109</v>
       </c>
       <c r="H2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>170</v>
@@ -1984,7 +1987,7 @@
         <v>147</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6">
@@ -2012,7 +2015,7 @@
         <v>85</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -2038,7 +2041,7 @@
         <v>87</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -2064,7 +2067,7 @@
         <v>89</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -2092,7 +2095,7 @@
         <v>112</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6">
@@ -2100,34 +2103,38 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>222</v>
+      </c>
       <c r="B8" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="E8" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" t="s">
         <v>220</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>222</v>
-      </c>
       <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="J8" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>11</v>
@@ -2148,11 +2155,11 @@
         <v>93</v>
       </c>
       <c r="H9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -2178,7 +2185,7 @@
         <v>100</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6">
@@ -2208,7 +2215,7 @@
         <v>104</v>
       </c>
       <c r="H11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6">
@@ -2238,7 +2245,7 @@
         <v>97</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6">
@@ -2268,7 +2275,7 @@
         <v>105</v>
       </c>
       <c r="H13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6">
@@ -2296,7 +2303,7 @@
         <v>154</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -2322,7 +2329,7 @@
         <v>116</v>
       </c>
       <c r="H15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6">
@@ -2352,7 +2359,7 @@
         <v>143</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6">
@@ -2382,7 +2389,7 @@
         <v>159</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6">
@@ -2394,7 +2401,7 @@
         <v>165</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>151</v>
@@ -2412,7 +2419,7 @@
         <v>150</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6">
@@ -2440,7 +2447,7 @@
         <v>120</v>
       </c>
       <c r="H19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6">
@@ -2468,7 +2475,7 @@
         <v>124</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>170</v>
@@ -2500,7 +2507,7 @@
         <v>44</v>
       </c>
       <c r="H21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6">
@@ -2530,7 +2537,7 @@
         <v>46</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6">
@@ -2560,7 +2567,7 @@
         <v>66</v>
       </c>
       <c r="H23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6">
@@ -2590,7 +2597,7 @@
         <v>48</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="6">
@@ -2620,7 +2627,7 @@
         <v>51</v>
       </c>
       <c r="H25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="6">
@@ -2650,7 +2657,7 @@
         <v>54</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6">
@@ -2680,7 +2687,7 @@
         <v>70</v>
       </c>
       <c r="H27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="6">
@@ -2710,7 +2717,7 @@
         <v>75</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6">
@@ -2740,7 +2747,7 @@
         <v>58</v>
       </c>
       <c r="H29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6">
@@ -2770,7 +2777,7 @@
         <v>77</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6">
@@ -2800,7 +2807,7 @@
         <v>81</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="6">
@@ -2812,7 +2819,7 @@
         <v>128</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="6" t="s">
@@ -2828,7 +2835,7 @@
         <v>127</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>171</v>
@@ -2856,7 +2863,7 @@
         <v>131</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>170</v>
@@ -2886,7 +2893,7 @@
         <v>133</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>170</v>
@@ -2916,7 +2923,7 @@
         <v>136</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>170</v>
@@ -2946,7 +2953,7 @@
         <v>139</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6">
@@ -2973,13 +2980,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B39">
         <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J39" s="13" t="str">
         <f>"Total: " &amp; SUM(J2:J37)</f>
@@ -2988,13 +2995,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B40">
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flipped all the parts to the TOP. TODO: change C17,C39 to 0402 size
</commit_message>
<xml_diff>
--- a/Sch/adc/zturn_adc.xlsx
+++ b/Sch/adc/zturn_adc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19356" windowHeight="9024"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19356" windowHeight="10308"/>
   </bookViews>
   <sheets>
     <sheet name="zturn_adc" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="221">
   <si>
     <t xml:space="preserve"> Value</t>
   </si>
@@ -681,23 +681,7 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t xml:space="preserve">Mount Top Side </t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Mount Bottom Side</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>SMD Parts Count</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>C4,C40,C46,C47,C53</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>All the other</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -870,6 +854,10 @@
   </si>
   <si>
     <t>R2,R3,R9,R10,R11,R27,R28</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>All the SMD parts are on the TOP side</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -1884,10 +1872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1927,13 +1915,13 @@
         <v>172</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>169</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1957,7 +1945,7 @@
         <v>109</v>
       </c>
       <c r="H2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>170</v>
@@ -1987,7 +1975,7 @@
         <v>147</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6">
@@ -2015,7 +2003,7 @@
         <v>85</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -2041,7 +2029,7 @@
         <v>87</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -2067,7 +2055,7 @@
         <v>89</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -2095,7 +2083,7 @@
         <v>112</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6">
@@ -2104,28 +2092,28 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="G8" t="s">
+        <v>216</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="G8" t="s">
-        <v>220</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>221</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6">
@@ -2134,7 +2122,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>11</v>
@@ -2155,7 +2143,7 @@
         <v>93</v>
       </c>
       <c r="H9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6">
@@ -2185,7 +2173,7 @@
         <v>100</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6">
@@ -2215,7 +2203,7 @@
         <v>104</v>
       </c>
       <c r="H11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6">
@@ -2245,7 +2233,7 @@
         <v>97</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6">
@@ -2275,7 +2263,7 @@
         <v>105</v>
       </c>
       <c r="H13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6">
@@ -2303,7 +2291,7 @@
         <v>154</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -2329,7 +2317,7 @@
         <v>116</v>
       </c>
       <c r="H15" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6">
@@ -2359,7 +2347,7 @@
         <v>143</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6">
@@ -2389,7 +2377,7 @@
         <v>159</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6">
@@ -2401,7 +2389,7 @@
         <v>165</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>151</v>
@@ -2419,7 +2407,7 @@
         <v>150</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6">
@@ -2447,7 +2435,7 @@
         <v>120</v>
       </c>
       <c r="H19" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6">
@@ -2475,7 +2463,7 @@
         <v>124</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>170</v>
@@ -2507,7 +2495,7 @@
         <v>44</v>
       </c>
       <c r="H21" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6">
@@ -2537,7 +2525,7 @@
         <v>46</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6">
@@ -2567,7 +2555,7 @@
         <v>66</v>
       </c>
       <c r="H23" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6">
@@ -2597,7 +2585,7 @@
         <v>48</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="6">
@@ -2627,7 +2615,7 @@
         <v>51</v>
       </c>
       <c r="H25" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="6">
@@ -2657,7 +2645,7 @@
         <v>54</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6">
@@ -2687,7 +2675,7 @@
         <v>70</v>
       </c>
       <c r="H27" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="6">
@@ -2717,7 +2705,7 @@
         <v>75</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6">
@@ -2747,7 +2735,7 @@
         <v>58</v>
       </c>
       <c r="H29" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6">
@@ -2777,7 +2765,7 @@
         <v>77</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6">
@@ -2807,7 +2795,7 @@
         <v>81</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="6">
@@ -2819,7 +2807,7 @@
         <v>128</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="6" t="s">
@@ -2835,7 +2823,7 @@
         <v>127</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>171</v>
@@ -2863,7 +2851,7 @@
         <v>131</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>170</v>
@@ -2893,7 +2881,7 @@
         <v>133</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>170</v>
@@ -2923,7 +2911,7 @@
         <v>136</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>170</v>
@@ -2953,7 +2941,7 @@
         <v>139</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6">
@@ -2980,28 +2968,11 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>174</v>
-      </c>
-      <c r="B39">
-        <v>98</v>
-      </c>
-      <c r="C39" t="s">
-        <v>178</v>
+        <v>220</v>
       </c>
       <c r="J39" s="13" t="str">
         <f>"Total: " &amp; SUM(J2:J37)</f>
         <v>Total: 103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>175</v>
-      </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Qty column to BOM. Add SMD attribute to ADC board
</commit_message>
<xml_diff>
--- a/Sch/adc/zturn_adc.xlsx
+++ b/Sch/adc/zturn_adc.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21264" windowHeight="8484"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8484"/>
   </bookViews>
   <sheets>
     <sheet name="zturn_adc_new" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="228">
   <si>
     <t>Reference</t>
   </si>
@@ -834,6 +834,18 @@
   </si>
   <si>
     <t>http://www.taitien.com/wp-content/uploads/2015/12/XO-0076_TX.pdf</t>
+  </si>
+  <si>
+    <t>Qty</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>SMD</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Total Components</t>
+    <phoneticPr fontId="18"/>
   </si>
 </sst>
 </file>
@@ -1813,11 +1825,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1827,14 +1839,15 @@
     <col min="3" max="3" width="27.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.44140625" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="66.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="66.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1851,22 +1864,25 @@
         <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1882,23 +1898,26 @@
       <c r="E2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
@@ -1914,21 +1933,24 @@
       <c r="E3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>73</v>
       </c>
@@ -1942,21 +1964,24 @@
       <c r="E4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7">
+        <v>3</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>63</v>
       </c>
@@ -1969,12 +1994,13 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="7" t="s">
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>72</v>
       </c>
@@ -1988,21 +2014,24 @@
       <c r="E6" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7">
+        <v>4</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>112</v>
       </c>
@@ -2018,21 +2047,24 @@
       <c r="E7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="7">
+        <v>9</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>120</v>
       </c>
@@ -2048,21 +2080,24 @@
       <c r="E8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="7">
+        <v>16</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>119</v>
       </c>
@@ -2078,21 +2113,24 @@
       <c r="E9" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="7">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>129</v>
       </c>
@@ -2108,21 +2146,24 @@
       <c r="E10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="7">
+        <v>4</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="I10" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>93</v>
       </c>
@@ -2138,21 +2179,24 @@
       <c r="E11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="7">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>94</v>
       </c>
@@ -2168,21 +2212,24 @@
       <c r="E12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="7">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="J12" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -2198,21 +2245,24 @@
       <c r="E13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I13" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
@@ -2228,21 +2278,24 @@
       <c r="E14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="J14" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>29</v>
       </c>
@@ -2258,21 +2311,24 @@
       <c r="E15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>60</v>
       </c>
@@ -2288,21 +2344,24 @@
       <c r="E16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="7">
+        <v>2</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="H16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="I16" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="J16" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>98</v>
       </c>
@@ -2318,21 +2377,24 @@
       <c r="E17" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="7">
+        <v>5</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="H17" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="I17" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="J17" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
@@ -2348,21 +2410,24 @@
       <c r="E18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="H18" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="I18" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="J18" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>95</v>
       </c>
@@ -2378,21 +2443,24 @@
       <c r="E19" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="7">
+        <v>2</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="H19" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="I19" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="J19" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>156</v>
       </c>
@@ -2408,21 +2476,24 @@
       <c r="E20" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="7">
+        <v>3</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="H20" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="I20" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="J20" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>88</v>
       </c>
@@ -2433,18 +2504,17 @@
         <v>54</v>
       </c>
       <c r="D21" s="9"/>
-      <c r="E21" s="7" t="s">
-        <v>46</v>
-      </c>
+      <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="7" t="s">
+      <c r="I21" s="7"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>84</v>
       </c>
@@ -2460,21 +2530,24 @@
       <c r="E22" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="7">
+        <v>3</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="H22" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="I22" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="J22" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J22" s="7"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>87</v>
       </c>
@@ -2490,21 +2563,24 @@
       <c r="E23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="7">
+        <v>6</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="H23" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="I23" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="J23" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J23" s="7"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>96</v>
       </c>
@@ -2520,21 +2596,24 @@
       <c r="E24" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="7">
+        <v>2</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="H24" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="I24" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="J24" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="J24" s="7"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>97</v>
       </c>
@@ -2550,21 +2629,24 @@
       <c r="E25" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="7">
+        <v>2</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="I25" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="J25" s="7"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>100</v>
       </c>
@@ -2580,21 +2662,24 @@
       <c r="E26" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="7">
+        <v>2</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="J26" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="J26" s="7"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>32</v>
       </c>
@@ -2610,21 +2695,24 @@
       <c r="E27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="7">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="I27" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="J27" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="J27" s="7"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>25</v>
       </c>
@@ -2640,21 +2728,24 @@
       <c r="E28" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="7">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="H28" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="J28" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J28" s="7"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>19</v>
       </c>
@@ -2670,21 +2761,24 @@
       <c r="E29" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="H29" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="I29" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="J29" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="J29" s="7"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>20</v>
       </c>
@@ -2700,23 +2794,26 @@
       <c r="E30" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="7">
+        <v>1</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="H30" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="I30" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="J30" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="J30" s="7" t="s">
+      <c r="K30" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>58</v>
       </c>
@@ -2732,21 +2829,24 @@
       <c r="E31" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="7">
+        <v>2</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="H31" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="I31" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="J31" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="J31" s="7"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>27</v>
       </c>
@@ -2762,21 +2862,24 @@
       <c r="E32" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="7">
+        <v>1</v>
+      </c>
+      <c r="G32" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="H32" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="H32" s="7" t="s">
+      <c r="I32" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="J32" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="J32" s="7"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>77</v>
       </c>
@@ -2792,23 +2895,26 @@
       <c r="E33" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="7">
+        <v>2</v>
+      </c>
+      <c r="G33" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="H33" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="H33" s="7" t="s">
+      <c r="I33" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="J33" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="J33" s="7" t="s">
+      <c r="K33" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>31</v>
       </c>
@@ -2824,21 +2930,24 @@
       <c r="E34" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="7">
+        <v>1</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="H34" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="I34" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="J34" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="J34" s="7"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>33</v>
       </c>
@@ -2854,21 +2963,24 @@
       <c r="E35" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="7">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="H35" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="I35" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="J35" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="J35" s="7"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>34</v>
       </c>
@@ -2884,23 +2996,26 @@
       <c r="E36" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="7">
+        <v>1</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="H36" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H36" s="7" t="s">
+      <c r="I36" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="J36" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="J36" s="7" t="s">
+      <c r="K36" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>59</v>
       </c>
@@ -2916,21 +3031,24 @@
       <c r="E37" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="7">
+        <v>2</v>
+      </c>
+      <c r="G37" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="H37" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="I37" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="J37" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="J37" s="7"/>
-    </row>
-    <row r="38" spans="1:10" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>36</v>
       </c>
@@ -2946,21 +3064,24 @@
       <c r="E38" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F38" s="7">
+        <v>1</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="H38" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="H38" s="10" t="s">
+      <c r="I38" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="J38" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J38" s="7"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>86</v>
       </c>
@@ -2976,19 +3097,40 @@
       <c r="E39" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="7">
+        <v>4</v>
+      </c>
+      <c r="G39" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="H39" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="I39" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="J39" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>227</v>
+      </c>
+      <c r="F41">
+        <f>SUM(F2:F39)</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>226</v>
+      </c>
+      <c r="F42">
+        <f>F41-F4-F6-F37-F21</f>
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>

</xml_diff>

<commit_message>
Add 2 test headers
</commit_message>
<xml_diff>
--- a/Sch/adc/zturn_adc.xlsx
+++ b/Sch/adc/zturn_adc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8484"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9960"/>
   </bookViews>
   <sheets>
     <sheet name="zturn_adc_new" sheetId="1" r:id="rId1"/>
@@ -265,10 +265,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>W1,W2,W3,W4</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>J1,J3,J4</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -845,6 +841,10 @@
   </si>
   <si>
     <t>Total Components</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>W1,W2,W3,W4,W5,W6</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -1828,8 +1828,8 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1858,13 +1858,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>43</v>
@@ -1890,10 +1890,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>46</v>
@@ -1902,19 +1902,19 @@
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>71</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1928,7 +1928,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>46</v>
@@ -1952,14 +1952,14 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>67</v>
@@ -1968,13 +1968,13 @@
         <v>3</v>
       </c>
       <c r="G4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>70</v>
@@ -2002,20 +2002,20 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>72</v>
+        <v>227</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>67</v>
       </c>
       <c r="F6" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>68</v>
@@ -2033,16 +2033,16 @@
     </row>
     <row r="7" spans="1:11" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>46</v>
@@ -2051,13 +2051,13 @@
         <v>9</v>
       </c>
       <c r="G7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>111</v>
-      </c>
       <c r="I7" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>71</v>
@@ -2066,16 +2066,16 @@
     </row>
     <row r="8" spans="1:11" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>46</v>
@@ -2084,22 +2084,22 @@
         <v>16</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>41</v>
@@ -2108,7 +2108,7 @@
         <v>47</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>46</v>
@@ -2117,31 +2117,31 @@
         <v>5</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>46</v>
@@ -2150,31 +2150,31 @@
         <v>4</v>
       </c>
       <c r="G10" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="I10" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>126</v>
-      </c>
       <c r="J10" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>46</v>
@@ -2183,31 +2183,31 @@
         <v>4</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="J11" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>46</v>
@@ -2216,16 +2216,16 @@
         <v>4</v>
       </c>
       <c r="G12" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="J12" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K12" s="7"/>
     </row>
@@ -2240,7 +2240,7 @@
         <v>47</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>46</v>
@@ -2249,16 +2249,16 @@
         <v>1</v>
       </c>
       <c r="G13" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>138</v>
-      </c>
       <c r="J13" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K13" s="7"/>
     </row>
@@ -2273,7 +2273,7 @@
         <v>47</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>46</v>
@@ -2282,16 +2282,16 @@
         <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="J14" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K14" s="7"/>
     </row>
@@ -2300,13 +2300,13 @@
         <v>29</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>46</v>
@@ -2315,16 +2315,16 @@
         <v>1</v>
       </c>
       <c r="G15" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I15" s="3" t="s">
+      <c r="J15" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="K15" s="7"/>
     </row>
@@ -2339,7 +2339,7 @@
         <v>53</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>46</v>
@@ -2354,16 +2354,16 @@
         <v>62</v>
       </c>
       <c r="I16" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="6">
         <v>22</v>
@@ -2372,7 +2372,7 @@
         <v>47</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>46</v>
@@ -2381,13 +2381,13 @@
         <v>5</v>
       </c>
       <c r="G17" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="I17" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>70</v>
@@ -2405,7 +2405,7 @@
         <v>47</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>46</v>
@@ -2414,13 +2414,13 @@
         <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>161</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>70</v>
@@ -2429,7 +2429,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="6">
         <v>25</v>
@@ -2438,7 +2438,7 @@
         <v>47</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>46</v>
@@ -2447,22 +2447,22 @@
         <v>2</v>
       </c>
       <c r="G19" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="H19" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>163</v>
-      </c>
       <c r="J19" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>8</v>
@@ -2471,7 +2471,7 @@
         <v>47</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>46</v>
@@ -2480,22 +2480,22 @@
         <v>3</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I20" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="J20" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>40</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>11</v>
@@ -2525,7 +2525,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>46</v>
@@ -2534,13 +2534,13 @@
         <v>3</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>70</v>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>11</v>
@@ -2558,7 +2558,7 @@
         <v>47</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>46</v>
@@ -2567,13 +2567,13 @@
         <v>6</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>70</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24" s="6">
         <v>25</v>
@@ -2591,7 +2591,7 @@
         <v>48</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>46</v>
@@ -2600,22 +2600,22 @@
         <v>2</v>
       </c>
       <c r="G24" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="H24" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>169</v>
-      </c>
       <c r="J24" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" s="6">
         <v>12</v>
@@ -2624,7 +2624,7 @@
         <v>48</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>46</v>
@@ -2633,22 +2633,22 @@
         <v>2</v>
       </c>
       <c r="G25" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="I25" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26" s="6">
         <v>0</v>
@@ -2657,7 +2657,7 @@
         <v>47</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>46</v>
@@ -2666,16 +2666,16 @@
         <v>2</v>
       </c>
       <c r="G26" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I26" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="J26" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K26" s="7"/>
     </row>
@@ -2690,7 +2690,7 @@
         <v>47</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>46</v>
@@ -2699,16 +2699,16 @@
         <v>1</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K27" s="7"/>
     </row>
@@ -2723,7 +2723,7 @@
         <v>47</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>46</v>
@@ -2732,13 +2732,13 @@
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="I28" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J28" s="8" t="s">
         <v>70</v>
@@ -2756,7 +2756,7 @@
         <v>47</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>46</v>
@@ -2765,16 +2765,16 @@
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I29" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="H29" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="J29" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K29" s="7"/>
     </row>
@@ -2786,31 +2786,31 @@
         <v>21</v>
       </c>
       <c r="C30" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>224</v>
-      </c>
       <c r="E30" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F30" s="7">
         <v>1</v>
       </c>
       <c r="G30" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="H30" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="I30" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>222</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>71</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -2821,25 +2821,25 @@
         <v>24</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>195</v>
-      </c>
       <c r="E31" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F31" s="7">
         <v>2</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H31" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="I31" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>71</v>
@@ -2854,64 +2854,64 @@
         <v>28</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F32" s="7">
         <v>1</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H32" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="I32" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="I32" s="7" t="s">
-        <v>199</v>
-      </c>
       <c r="J32" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K32" s="7"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F33" s="7">
         <v>2</v>
       </c>
       <c r="G33" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="H33" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="H33" s="7" t="s">
+      <c r="I33" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="I33" s="7" t="s">
-        <v>208</v>
-      </c>
       <c r="J33" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -2919,13 +2919,13 @@
         <v>31</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>46</v>
@@ -2934,16 +2934,16 @@
         <v>1</v>
       </c>
       <c r="G34" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I34" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H34" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="I34" s="7" t="s">
+      <c r="J34" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>192</v>
       </c>
       <c r="K34" s="7"/>
     </row>
@@ -2952,13 +2952,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>51</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>46</v>
@@ -2967,16 +2967,16 @@
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>62</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K35" s="7"/>
     </row>
@@ -2988,10 +2988,10 @@
         <v>35</v>
       </c>
       <c r="C36" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>203</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>204</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>46</v>
@@ -3000,19 +3000,19 @@
         <v>1</v>
       </c>
       <c r="G36" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H36" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="H36" s="10" t="s">
+      <c r="I36" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>71</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -3026,25 +3026,25 @@
         <v>18</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F37" s="7">
         <v>2</v>
       </c>
       <c r="G37" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H37" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="I37" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I37" s="7" t="s">
+      <c r="J37" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>108</v>
       </c>
       <c r="K37" s="7"/>
     </row>
@@ -3059,7 +3059,7 @@
         <v>38</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>46</v>
@@ -3068,13 +3068,13 @@
         <v>1</v>
       </c>
       <c r="G38" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H38" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="H38" s="7" t="s">
+      <c r="I38" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>83</v>
       </c>
       <c r="J38" s="8" t="s">
         <v>70</v>
@@ -3083,16 +3083,16 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>52</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>46</v>
@@ -3101,31 +3101,31 @@
         <v>4</v>
       </c>
       <c r="G39" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="I39" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="I39" s="7" t="s">
-        <v>215</v>
-      </c>
       <c r="J39" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K39" s="7"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E41" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F41">
         <f>SUM(F2:F39)</f>
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F42">
         <f>F41-F4-F6-F37-F21</f>

</xml_diff>